<commit_message>
Add menu for Edit/Remove from Products table
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sara\IdeaProjects\elderberry-inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sara\IdeaProjects\Project\elderberry-inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEC756A-196C-4FCC-ACC7-6DFCA51B4681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CEE2E2-F6F2-41F8-A05B-7F8E0ECF877A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2FB9CC1B-55EA-4AB0-A71D-09585E9EFDF3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>amount</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>backet</t>
-  </si>
-  <si>
-    <t>pic</t>
   </si>
   <si>
     <t>N-have</t>
@@ -188,12 +185,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D6FD1A-161B-4F93-974F-1B4D5B2BD463}">
-  <dimension ref="A2:G11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,26 +524,25 @@
     <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E1" s="5"/>
+    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -559,17 +557,19 @@
       <c r="D3" s="2">
         <v>10</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2">
-        <v>2</v>
-      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -577,7 +577,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -585,7 +585,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -613,16 +613,16 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -669,15 +669,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D420E07-FDA5-4EC0-A51C-98BED7948BE3}">
-  <dimension ref="B2:D6"/>
+  <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -687,8 +690,11 @@
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -698,8 +704,11 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -709,8 +718,9 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -720,8 +730,9 @@
       <c r="D5" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>1</v>
       </c>
@@ -731,6 +742,7 @@
       <c r="D6" s="2">
         <v>3</v>
       </c>
+      <c r="E6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>